<commit_message>
Final Submission for Milestone 1
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B91B6E-FCDB-4984-837B-B182A74227CB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDC79FC-4971-41CC-9C5F-D86E2C98FC09}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="99">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -313,6 +313,12 @@
   </si>
   <si>
     <t>Student Git Address: https://github.com/cphall/PPIV-Project.git</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -902,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,15 +1023,19 @@
       <c r="D4" s="5">
         <v>2</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G4" s="16">
         <f t="shared" ref="G4:G68" si="0" xml:space="preserve"> IF(EXACT(F4,"X"),IF(EXACT(E4,"I"),$B4,IF(EXACT(E4,"II"),$C4,IF(EXACT(E4,"III"),$D4,0))),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H4" s="17">
         <f>IF(SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87))</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87))</f>
@@ -1041,7 +1051,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1166,7 +1176,7 @@
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
@@ -1835,11 +1845,15 @@
       <c r="D37" s="5">
         <v>1</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="3"/>
+      <c r="E37" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G37" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -2274,11 +2288,15 @@
       <c r="D56" s="5">
         <v>2</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="3"/>
+      <c r="E56" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G56" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -2911,7 +2929,9 @@
       <c r="B86" s="6">
         <v>2</v>
       </c>
-      <c r="C86" s="3"/>
+      <c r="C86" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
       <c r="F86" s="5"/>
@@ -2929,7 +2949,9 @@
       <c r="B87" s="6">
         <v>1</v>
       </c>
-      <c r="C87" s="3"/>
+      <c r="C87" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
       <c r="F87" s="5"/>
@@ -3064,7 +3086,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Fixed the rendering issue with the previous camera. Need to still implement proper rotation of the camera.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDC79FC-4971-41CC-9C5F-D86E2C98FC09}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7034489D-3617-4996-9974-040B7D4F8924}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="100">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -908,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1042,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
@@ -1051,7 +1054,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1180,7 +1183,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1481,11 +1484,15 @@
       <c r="D21" s="5">
         <v>2</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G21" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
@@ -2445,11 +2452,15 @@
       <c r="D63" s="5">
         <v>1</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="3"/>
+      <c r="E63" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
@@ -3086,7 +3097,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Added pixel and vertex shader. Got a second cube rendering and stationary. Skybox is almost applied.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F5D290-D67D-4152-A556-05F3AF343A43}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6D0ABD-580A-4C0D-A81F-62609412FE06}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,11 +1047,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87)  &gt; 18, SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87) - 18,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) - 18,0)</f>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
@@ -2561,11 +2561,15 @@
       <c r="D67" s="5">
         <v>1</v>
       </c>
-      <c r="E67" s="2"/>
-      <c r="F67" s="3"/>
+      <c r="E67" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G67" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>

</xml_diff>

<commit_message>
Updated rubric and added a read me for camera controls.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6D0ABD-580A-4C0D-A81F-62609412FE06}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AFA199-DC64-4AD5-BD39-2EFE117C449A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="99">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -908,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,11 +1047,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1108,7 +1108,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87)  &gt; 18, SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87) - 18,0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) - 18,0)</f>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
@@ -1560,11 +1560,15 @@
       <c r="D24" s="5">
         <v>3</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
+      <c r="E24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G24" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
@@ -3106,7 +3110,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Updated project rubric for next milestone. Started programming for adjusting screen size / fullscreen.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4AFA199-DC64-4AD5-BD39-2EFE117C449A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C091B568-B8DE-4496-8CA4-AE2CD69DFA16}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="100">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
   </si>
 </sst>
 </file>
@@ -908,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F67" sqref="F67"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,7 +1042,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87))</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
@@ -1047,11 +1050,11 @@
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1108,7 +1111,7 @@
       </c>
       <c r="H6" s="17">
         <f>IF(SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87)  &gt; 18, SUMIF(E4:E84,"=I",G4:G84) + SUMIF(C86:C87, "X",B86:B87) - 18,0)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I6" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) - 18,0)</f>
@@ -1180,7 +1183,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1241,7 +1244,7 @@
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
@@ -1561,7 +1564,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>97</v>
@@ -2956,7 +2959,9 @@
       <c r="C86" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D86" s="3"/>
+      <c r="D86" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E86" s="3"/>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
@@ -2976,7 +2981,9 @@
       <c r="C87" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D87" s="3"/>
+      <c r="D87" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E87" s="3"/>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
@@ -3110,7 +3117,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Fullscreen implemented. Issues with image distortion.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15357FD0-7F0C-4947-BD78-998416588ACB}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-470" windowWidth="25440" windowHeight="15990"/>
+    <workbookView xWindow="0" yWindow="-465" windowWidth="25440" windowHeight="12255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="179017" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -329,7 +330,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -910,28 +911,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.453125" customWidth="1"/>
-    <col min="2" max="2" width="25.453125" customWidth="1"/>
+    <col min="1" max="1" width="106.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="6" width="25.453125" customWidth="1"/>
-    <col min="7" max="7" width="25.54296875" customWidth="1"/>
-    <col min="8" max="9" width="25.81640625" customWidth="1"/>
-    <col min="10" max="10" width="24.54296875" customWidth="1"/>
-    <col min="11" max="11" width="24.453125" customWidth="1"/>
-    <col min="12" max="12" width="24.1796875" customWidth="1"/>
-    <col min="13" max="14" width="9.1796875" customWidth="1"/>
+    <col min="4" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="8" max="9" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>95</v>
       </c>
@@ -947,7 +948,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>96</v>
       </c>
@@ -985,7 +986,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>87</v>
       </c>
@@ -1044,7 +1045,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=II",G4:G84) + SUMIF(D86:D87, "X",B86:B87))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
@@ -1056,10 +1057,10 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>84</v>
       </c>
@@ -1092,7 +1093,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>85</v>
       </c>
@@ -1129,7 +1130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>41</v>
       </c>
@@ -1160,7 +1161,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>42</v>
       </c>
@@ -1185,7 +1186,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1194,7 +1195,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>43</v>
       </c>
@@ -1225,7 +1226,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>44</v>
       </c>
@@ -1259,7 +1260,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>54</v>
       </c>
@@ -1284,7 +1285,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>62</v>
       </c>
@@ -1309,7 +1310,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>93</v>
       </c>
@@ -1334,7 +1335,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>94</v>
       </c>
@@ -1359,7 +1360,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>50</v>
       </c>
@@ -1384,7 +1385,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1401,7 +1402,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>56</v>
       </c>
@@ -1420,7 +1421,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -1437,7 +1438,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1454,7 +1455,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>10</v>
       </c>
@@ -1473,7 +1474,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>39</v>
       </c>
@@ -1502,7 +1503,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>55</v>
       </c>
@@ -1527,7 +1528,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>40</v>
       </c>
@@ -1552,7 +1553,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>38</v>
       </c>
@@ -1581,7 +1582,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
         <v>49</v>
       </c>
@@ -1606,7 +1607,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1623,7 +1624,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>88</v>
       </c>
@@ -1642,7 +1643,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>92</v>
       </c>
@@ -1667,7 +1668,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>74</v>
       </c>
@@ -1692,7 +1693,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>76</v>
       </c>
@@ -1717,7 +1718,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>75</v>
       </c>
@@ -1742,7 +1743,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>77</v>
       </c>
@@ -1767,7 +1768,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>78</v>
       </c>
@@ -1792,7 +1793,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1809,7 +1810,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1826,7 +1827,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>58</v>
       </c>
@@ -1845,7 +1846,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>91</v>
       </c>
@@ -1874,7 +1875,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>90</v>
       </c>
@@ -1899,7 +1900,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>86</v>
       </c>
@@ -1924,7 +1925,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>34</v>
       </c>
@@ -1949,7 +1950,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>48</v>
       </c>
@@ -1974,7 +1975,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>35</v>
       </c>
@@ -1999,7 +2000,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>36</v>
       </c>
@@ -2024,7 +2025,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>59</v>
       </c>
@@ -2049,7 +2050,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>37</v>
       </c>
@@ -2074,7 +2075,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>82</v>
       </c>
@@ -2099,7 +2100,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="22"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2116,7 +2117,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2133,7 +2134,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>8</v>
       </c>
@@ -2152,7 +2153,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>89</v>
       </c>
@@ -2177,7 +2178,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>51</v>
       </c>
@@ -2202,7 +2203,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>60</v>
       </c>
@@ -2227,7 +2228,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>83</v>
       </c>
@@ -2252,7 +2253,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -2269,7 +2270,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>7</v>
       </c>
@@ -2288,7 +2289,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>45</v>
       </c>
@@ -2317,7 +2318,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>73</v>
       </c>
@@ -2330,11 +2331,15 @@
       <c r="D57" s="5">
         <v>2</v>
       </c>
-      <c r="E57" s="2"/>
-      <c r="F57" s="3"/>
+      <c r="E57" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G57" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2342,7 +2347,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>79</v>
       </c>
@@ -2367,7 +2372,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>52</v>
       </c>
@@ -2392,7 +2397,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -2409,7 +2414,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -2426,7 +2431,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>6</v>
       </c>
@@ -2445,7 +2450,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>80</v>
       </c>
@@ -2474,7 +2479,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>81</v>
       </c>
@@ -2503,7 +2508,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>63</v>
       </c>
@@ -2532,7 +2537,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>64</v>
       </c>
@@ -2557,7 +2562,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>65</v>
       </c>
@@ -2586,7 +2591,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="21" t="s">
         <v>61</v>
       </c>
@@ -2611,7 +2616,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>53</v>
       </c>
@@ -2636,7 +2641,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2653,7 +2658,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2670,7 +2675,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>5</v>
       </c>
@@ -2689,7 +2694,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>0</v>
       </c>
@@ -2714,7 +2719,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
@@ -2731,7 +2736,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="11"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
@@ -2748,7 +2753,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>69</v>
       </c>
@@ -2767,7 +2772,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>70</v>
       </c>
@@ -2788,7 +2793,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>72</v>
       </c>
@@ -2809,7 +2814,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>71</v>
       </c>
@@ -2834,7 +2839,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="11" t="s">
         <v>67</v>
       </c>
@@ -2855,7 +2860,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
         <v>66</v>
       </c>
@@ -2876,7 +2881,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
         <v>68</v>
       </c>
@@ -2897,7 +2902,7 @@
       <c r="K82" s="5"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2914,7 +2919,7 @@
       <c r="K83" s="5"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2931,7 +2936,7 @@
       <c r="K84" s="5"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>32</v>
       </c>
@@ -2955,7 +2960,7 @@
       <c r="K85" s="6"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
         <v>18</v>
       </c>
@@ -2977,7 +2982,7 @@
       <c r="K86" s="6"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
         <v>29</v>
       </c>
@@ -2999,7 +3004,7 @@
       <c r="K87" s="6"/>
       <c r="L87" s="5"/>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
@@ -3013,7 +3018,7 @@
       <c r="K88" s="6"/>
       <c r="L88" s="5"/>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="11"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
@@ -3027,78 +3032,78 @@
       <c r="K89" s="5"/>
       <c r="L89" s="5"/>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="12"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="12"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="12"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="13"/>
     </row>
   </sheetData>
@@ -3123,7 +3128,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3162,18 +3167,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C86:E87 F4:F84">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C86:E87 F4:F84" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>IF(EXACT(C4,"X"),TRUE,FALSE)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D83:D84 D48:D81 B48:C84 B3:D47">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D83:D84 D48:D81 B48:C84 B3:D47" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D82">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D82" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>1</formula1>
       <formula2>6</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E84">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E84" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>IF(EXACT(E4,"I"),TRUE,IF(EXACT(E4,"II"),TRUE,IF(EXACT(E4,"III"),TRUE,FALSE)))</formula1>
     </dataValidation>
   </dataValidations>
@@ -3188,12 +3193,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3205,12 +3210,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Got all objects drawn and setup multiple viewports. Have point light code setup in pixel shader and main. Further work needed to get points.
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51080EB-8E4F-4A55-853C-27524CC6339E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A416DD8-6443-4172-BCCE-97AFC465CC0A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="-465" windowWidth="19200" windowHeight="7290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="101">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
@@ -911,8 +914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1049,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87) &gt; 18, 18, SUMIF(E4:E84,"=III",G4:G84) + SUMIF(E86:E87, "X",B86:B87))</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1054,7 +1057,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G84) + SUMIF(C86:C87, "X",B86:B87) + SUMIF(D86:D87, "X",B86:B87) + SUMIF(E86:E87, "X",B86:B87)</f>
-        <v>28</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1070,11 +1073,15 @@
       <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1140,11 +1147,15 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
+      <c r="E7" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>23</v>
@@ -1171,11 +1182,15 @@
       <c r="D8" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3"/>
+      <c r="E8" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8" s="18">
         <f>H4+IF(H4 &lt; 18, IF(K4+H4 &gt; 18, 18- H4, K4),0)</f>
@@ -1187,7 +1202,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1205,11 +1220,15 @@
       <c r="D9" s="5">
         <v>1</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="19" t="s">
         <v>26</v>
@@ -2601,11 +2620,15 @@
       <c r="D68" s="5">
         <v>4</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="3"/>
+      <c r="E68" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G68" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
@@ -2820,11 +2843,15 @@
       <c r="D79" s="5">
         <v>4</v>
       </c>
-      <c r="E79" s="2"/>
-      <c r="F79" s="3"/>
+      <c r="E79" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="G79" s="16">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
@@ -2966,7 +2993,9 @@
       <c r="D86" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E86" s="3"/>
+      <c r="E86" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
@@ -2988,7 +3017,9 @@
       <c r="D87" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E87" s="3"/>
+      <c r="E87" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="F87" s="5"/>
       <c r="G87" s="5"/>
       <c r="H87" s="5"/>
@@ -3121,7 +3152,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>